<commit_message>
texts updated, some test added 19 04 22
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Study\DiplomMQA\fmh-android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127CBC4F-1DE8-42BC-BC0A-12F0093E055A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A9D01D-CD25-492B-9E5E-534ED132561F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>Проверка</t>
   </si>
@@ -82,6 +82,69 @@
   </si>
   <si>
     <t>Вклладка "About" отображается корректно</t>
+  </si>
+  <si>
+    <t>Экран Авторизация:</t>
+  </si>
+  <si>
+    <t>Элементы экрана отображаются</t>
+  </si>
+  <si>
+    <t>Поля экрана доступны для ввода данных, кнопки кликабельны</t>
+  </si>
+  <si>
+    <t>Экран Главного меню:</t>
+  </si>
+  <si>
+    <t>Топлайн клакабелен, кнопки кликабельны</t>
+  </si>
+  <si>
+    <t>Экран Фильтр новостей:</t>
+  </si>
+  <si>
+    <t>Экран Контрольная панель новостей:</t>
+  </si>
+  <si>
+    <t>Ссылки на экране кликабельны и открываются, кнопки кликабельны</t>
+  </si>
+  <si>
+    <t>Экран Фильтрация Жалоб:</t>
+  </si>
+  <si>
+    <t>Экран Жалобы:</t>
+  </si>
+  <si>
+    <t>Экран О нас:</t>
+  </si>
+  <si>
+    <t>Экран Добавление новости:</t>
+  </si>
+  <si>
+    <t>Экран Новости:</t>
+  </si>
+  <si>
+    <t>Кнопки кликабельны, чек-боксы работают</t>
+  </si>
+  <si>
+    <t>Экран Добавление жалобы:</t>
+  </si>
+  <si>
+    <t>Экран Редактирование жалобы:</t>
+  </si>
+  <si>
+    <t>Кнопки кликабельны</t>
+  </si>
+  <si>
+    <t>Экран Цитаты:</t>
+  </si>
+  <si>
+    <t>Экран Добавление комментария к жалобе:</t>
+  </si>
+  <si>
+    <t>Экран Редактирования комментария к жалобе:</t>
+  </si>
+  <si>
+    <t>Экран Редактирование  новости:</t>
   </si>
 </sst>
 </file>
@@ -429,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,103 +512,103 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -554,6 +617,261 @@
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>